<commit_message>
Feat: New WeaponSystem & Arm Weapon 모델 3종 추가
</commit_message>
<xml_diff>
--- a/Assets/@Project/Scripts/Data/RawData/PartDbSheet.xlsx
+++ b/Assets/@Project/Scripts/Data/RawData/PartDbSheet.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27525"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27528"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{061249B2-DD8D-45F9-B9EC-331D65AE8654}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F5F2A6B9-66EC-49A6-A2B1-6EDDBABD75C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="59">
   <si>
     <t>dev_ID</t>
   </si>
@@ -174,6 +174,24 @@
     <t>TEST WEAPON_ARM_02</t>
   </si>
   <si>
+    <t>Arm_03</t>
+  </si>
+  <si>
+    <t>Prefabs/Parts/Weapon_Arm/Weapon_Arm_03</t>
+  </si>
+  <si>
+    <t>TEST WEAPON_ARM_03</t>
+  </si>
+  <si>
+    <t>Arm_04</t>
+  </si>
+  <si>
+    <t>Prefabs/Parts/Weapon_Arm/Weapon_Arm_04</t>
+  </si>
+  <si>
+    <t>TEST WEAPON_ARM_04</t>
+  </si>
+  <si>
     <t>Shoulder_01</t>
   </si>
   <si>
@@ -184,6 +202,9 @@
   </si>
   <si>
     <t>Weapon_Shoulder</t>
+  </si>
+  <si>
+    <t>Prefabs/Projectiles/PlayerBullet/Bullet_Missile_01</t>
   </si>
   <si>
     <t>Shoulder_02</t>
@@ -612,10 +633,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T20"/>
+  <dimension ref="A1:T22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+      <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -990,22 +1011,22 @@
         <v>42</v>
       </c>
       <c r="O6" s="3">
+        <v>5</v>
+      </c>
+      <c r="P6" s="3">
+        <v>25</v>
+      </c>
+      <c r="Q6" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="R6" s="3">
+        <v>3</v>
+      </c>
+      <c r="S6" s="3">
         <v>1</v>
       </c>
-      <c r="P6" s="3">
+      <c r="T6" s="3">
         <v>2</v>
-      </c>
-      <c r="Q6" s="3">
-        <v>3</v>
-      </c>
-      <c r="R6" s="3">
-        <v>4</v>
-      </c>
-      <c r="S6" s="3">
-        <v>5</v>
-      </c>
-      <c r="T6" s="3">
-        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:20" s="3" customFormat="1">
@@ -1072,7 +1093,7 @@
     </row>
     <row r="8" spans="1:20" s="3" customFormat="1">
       <c r="A8" s="3">
-        <v>10004001</v>
+        <v>10003003</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>46</v>
@@ -1087,13 +1108,13 @@
         <v>29</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="G8" s="3">
-        <v>120</v>
+        <v>275</v>
       </c>
       <c r="H8" s="3">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I8" s="3">
         <v>0</v>
@@ -1114,48 +1135,48 @@
         <v>42</v>
       </c>
       <c r="O8" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P8" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Q8" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="R8" s="3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="S8" s="3">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="T8" s="3">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:20" s="3" customFormat="1">
       <c r="A9" s="3">
-        <v>10004002</v>
+        <v>10003004</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="D9" s="3" t="s">
         <v>51</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>48</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>29</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="G9" s="3">
-        <v>200</v>
+        <v>275</v>
       </c>
       <c r="H9" s="3">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I9" s="3">
         <v>0</v>
@@ -1176,26 +1197,148 @@
         <v>42</v>
       </c>
       <c r="O9" s="3">
+        <v>2</v>
+      </c>
+      <c r="P9" s="3">
+        <v>3</v>
+      </c>
+      <c r="Q9" s="3">
+        <v>4</v>
+      </c>
+      <c r="R9" s="3">
+        <v>5</v>
+      </c>
+      <c r="S9" s="3">
+        <v>6</v>
+      </c>
+      <c r="T9" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" s="3" customFormat="1">
+      <c r="A10" s="3">
+        <v>10004001</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G10" s="3">
+        <v>120</v>
+      </c>
+      <c r="H10" s="3">
+        <v>5</v>
+      </c>
+      <c r="I10" s="3">
+        <v>0</v>
+      </c>
+      <c r="J10" s="3">
+        <v>0</v>
+      </c>
+      <c r="K10" s="3">
+        <v>0</v>
+      </c>
+      <c r="L10" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="M10" s="3">
+        <v>0</v>
+      </c>
+      <c r="N10" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="O10" s="3">
+        <v>5</v>
+      </c>
+      <c r="P10" s="3">
+        <v>15</v>
+      </c>
+      <c r="Q10" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="R10" s="3">
+        <v>5</v>
+      </c>
+      <c r="S10" s="3">
+        <v>5</v>
+      </c>
+      <c r="T10" s="3">
         <v>1</v>
       </c>
-      <c r="P9" s="3">
+    </row>
+    <row r="11" spans="1:20" s="3" customFormat="1">
+      <c r="A11" s="3">
+        <v>10004002</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G11" s="3">
+        <v>200</v>
+      </c>
+      <c r="H11" s="3">
+        <v>5</v>
+      </c>
+      <c r="I11" s="3">
+        <v>0</v>
+      </c>
+      <c r="J11" s="3">
+        <v>0</v>
+      </c>
+      <c r="K11" s="3">
+        <v>0</v>
+      </c>
+      <c r="L11" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="M11" s="3">
+        <v>0</v>
+      </c>
+      <c r="N11" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="O11" s="3">
         <v>1</v>
       </c>
-      <c r="Q9" s="3">
+      <c r="P11" s="3">
         <v>1</v>
       </c>
-      <c r="R9" s="3">
+      <c r="Q11" s="3">
         <v>1</v>
       </c>
-      <c r="S9" s="3">
+      <c r="R11" s="3">
         <v>1</v>
       </c>
-      <c r="T9" s="3">
+      <c r="S11" s="3">
         <v>1</v>
       </c>
+      <c r="T11" s="3">
+        <v>1</v>
+      </c>
     </row>
-    <row r="10" spans="1:20" s="3" customFormat="1"/>
-    <row r="11" spans="1:20" s="3" customFormat="1"/>
     <row r="12" spans="1:20" s="3" customFormat="1"/>
     <row r="13" spans="1:20" s="3" customFormat="1"/>
     <row r="14" spans="1:20" s="3" customFormat="1"/>
@@ -1204,7 +1347,9 @@
     <row r="17" s="3" customFormat="1"/>
     <row r="18" s="3" customFormat="1"/>
     <row r="19" s="3" customFormat="1"/>
-    <row r="20" s="4" customFormat="1"/>
+    <row r="20" s="3" customFormat="1"/>
+    <row r="21" s="3" customFormat="1"/>
+    <row r="22" s="4" customFormat="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Feat: MainScene UI 개선(진행중)
</commit_message>
<xml_diff>
--- a/Assets/@Project/Scripts/Data/RawData/PartDbSheet.xlsx
+++ b/Assets/@Project/Scripts/Data/RawData/PartDbSheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27528"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ADE2C7E3-4DFC-4FE3-BA08-D4D375787A01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{478779E2-8A92-45C0-B4FD-8637983234A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="70">
   <si>
     <t>dev_ID</t>
   </si>
@@ -40,6 +40,9 @@
   </si>
   <si>
     <t>prefab_Path</t>
+  </si>
+  <si>
+    <t>sprite_Path</t>
   </si>
   <si>
     <t>display_Name</t>
@@ -156,6 +159,9 @@
     <t>Prefabs/Parts/Weapon_Arm/Weapon_Arm_01</t>
   </si>
   <si>
+    <t>Images/Weapon_01</t>
+  </si>
+  <si>
     <t>CA-STD</t>
   </si>
   <si>
@@ -173,6 +179,9 @@
   </si>
   <si>
     <t>Prefabs/Parts/Weapon_Arm/Weapon_Arm_02</t>
+  </si>
+  <si>
+    <t>Images/Weapon_02</t>
   </si>
   <si>
     <t>GA-S</t>
@@ -192,6 +201,9 @@
     <t>Prefabs/Parts/Weapon_Arm/Weapon_Arm_03</t>
   </si>
   <si>
+    <t>Images/Weapon_03</t>
+  </si>
+  <si>
     <t>LC-S</t>
   </si>
   <si>
@@ -204,6 +216,9 @@
   </si>
   <si>
     <t>Prefabs/Parts/Weapon_Arm/Weapon_Arm_04</t>
+  </si>
+  <si>
+    <t>Images/Weapon_04</t>
   </si>
   <si>
     <t>CA-AP</t>
@@ -660,10 +675,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T22"/>
+  <dimension ref="A1:U22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -671,20 +686,21 @@
     <col min="1" max="1" width="9.875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.125" customWidth="1"/>
     <col min="3" max="3" width="49.25" customWidth="1"/>
-    <col min="4" max="4" width="25.875" customWidth="1"/>
-    <col min="5" max="5" width="47.875" customWidth="1"/>
-    <col min="6" max="6" width="17.375" customWidth="1"/>
-    <col min="10" max="10" width="13.125" customWidth="1"/>
-    <col min="11" max="11" width="13" customWidth="1"/>
-    <col min="13" max="13" width="16.375" customWidth="1"/>
-    <col min="14" max="14" width="46.25" customWidth="1"/>
-    <col min="16" max="16" width="14.5" customWidth="1"/>
-    <col min="18" max="18" width="14.625" customWidth="1"/>
-    <col min="19" max="19" width="18.5" customWidth="1"/>
-    <col min="20" max="20" width="15.125" customWidth="1"/>
+    <col min="4" max="4" width="28" customWidth="1"/>
+    <col min="5" max="5" width="25.875" customWidth="1"/>
+    <col min="6" max="6" width="47.875" customWidth="1"/>
+    <col min="7" max="7" width="17.375" customWidth="1"/>
+    <col min="11" max="11" width="13.125" customWidth="1"/>
+    <col min="12" max="12" width="13" customWidth="1"/>
+    <col min="14" max="14" width="16.375" customWidth="1"/>
+    <col min="15" max="15" width="46.25" customWidth="1"/>
+    <col min="17" max="17" width="14.5" customWidth="1"/>
+    <col min="19" max="19" width="14.625" customWidth="1"/>
+    <col min="20" max="20" width="18.5" customWidth="1"/>
+    <col min="21" max="21" width="15.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="1" customFormat="1">
+    <row r="1" spans="1:21" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -745,34 +761,35 @@
       <c r="T1" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="2" spans="1:20" s="2" customFormat="1" ht="33">
+    <row r="2" spans="1:21" s="2" customFormat="1" ht="33">
       <c r="A2" s="2">
         <v>10001001</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="D2" s="5"/>
+      <c r="E2" s="2" t="s">
         <v>23</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="2">
         <v>2300</v>
       </c>
-      <c r="H2" s="2">
+      <c r="I2" s="2">
         <v>250</v>
-      </c>
-      <c r="I2" s="2">
-        <v>5</v>
       </c>
       <c r="J2" s="2">
         <v>5</v>
@@ -780,17 +797,17 @@
       <c r="K2" s="2">
         <v>5</v>
       </c>
-      <c r="L2" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="M2" s="2">
-        <v>0</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="O2" s="2">
-        <v>0</v>
+      <c r="L2" s="2">
+        <v>5</v>
+      </c>
+      <c r="M2" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="N2" s="2">
+        <v>0</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="P2" s="2">
         <v>0</v>
@@ -807,52 +824,52 @@
       <c r="T2" s="2">
         <v>0</v>
       </c>
+      <c r="U2" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:20" s="2" customFormat="1">
+    <row r="3" spans="1:21" s="2" customFormat="1">
       <c r="A3" s="2">
         <v>10001002</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3" s="2" t="s">
         <v>28</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>29</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G3" s="2">
+        <v>30</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" s="2">
         <v>10000</v>
       </c>
-      <c r="H3" s="2">
-        <v>1</v>
-      </c>
-      <c r="I3" s="6">
-        <v>1000</v>
-      </c>
-      <c r="J3" s="2">
+      <c r="I3" s="2">
+        <v>1</v>
+      </c>
+      <c r="J3" s="6">
         <v>1000</v>
       </c>
       <c r="K3" s="2">
         <v>1000</v>
       </c>
-      <c r="L3" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="M3" s="2">
-        <v>0</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="O3" s="2">
-        <v>0</v>
+      <c r="L3" s="2">
+        <v>1000</v>
+      </c>
+      <c r="M3" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="N3" s="2">
+        <v>0</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="P3" s="2">
         <v>0</v>
@@ -869,52 +886,53 @@
       <c r="T3" s="2">
         <v>0</v>
       </c>
+      <c r="U3" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:20" s="2" customFormat="1" ht="49.5">
+    <row r="4" spans="1:21" s="2" customFormat="1" ht="49.5">
       <c r="A4" s="2">
         <v>10002001</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D4" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="D4" s="5"/>
+      <c r="E4" s="2" t="s">
         <v>33</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H4" s="2">
         <v>3000</v>
       </c>
-      <c r="H4" s="2">
+      <c r="I4" s="2">
         <v>150</v>
       </c>
-      <c r="I4" s="2">
-        <v>0</v>
-      </c>
       <c r="J4" s="2">
         <v>0</v>
       </c>
       <c r="K4" s="2">
         <v>0</v>
       </c>
-      <c r="L4" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="M4" s="2">
+      <c r="L4" s="2">
+        <v>0</v>
+      </c>
+      <c r="M4" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="N4" s="2">
         <v>3</v>
       </c>
-      <c r="N4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="O4" s="2">
-        <v>0</v>
+      <c r="O4" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="P4" s="2">
         <v>0</v>
@@ -931,34 +949,34 @@
       <c r="T4" s="2">
         <v>0</v>
       </c>
+      <c r="U4" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:20" s="2" customFormat="1">
+    <row r="5" spans="1:21" s="2" customFormat="1">
       <c r="A5" s="2">
         <v>10002002</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="G5" s="2">
+      <c r="H5" s="2">
         <v>10000</v>
       </c>
-      <c r="H5" s="2">
-        <v>1</v>
-      </c>
       <c r="I5" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J5" s="2">
         <v>0</v>
@@ -966,17 +984,17 @@
       <c r="K5" s="2">
         <v>0</v>
       </c>
-      <c r="L5" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="M5" s="2">
+      <c r="L5" s="2">
+        <v>0</v>
+      </c>
+      <c r="M5" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="N5" s="2">
         <v>1000</v>
       </c>
-      <c r="N5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="O5" s="2">
-        <v>0</v>
+      <c r="O5" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="P5" s="2">
         <v>0</v>
@@ -993,362 +1011,374 @@
       <c r="T5" s="2">
         <v>0</v>
       </c>
+      <c r="U5" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:20" s="3" customFormat="1" ht="33">
+    <row r="6" spans="1:21" s="3" customFormat="1" ht="33">
       <c r="A6" s="3">
         <v>10003001</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D6" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="D6" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="E6" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="G6" s="3">
+      <c r="F6" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H6" s="3">
         <v>350</v>
       </c>
-      <c r="H6" s="3">
+      <c r="I6" s="3">
         <v>5</v>
       </c>
-      <c r="I6" s="3">
-        <v>0</v>
-      </c>
       <c r="J6" s="3">
         <v>0</v>
       </c>
       <c r="K6" s="3">
         <v>0</v>
       </c>
-      <c r="L6" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="M6" s="3">
-        <v>0</v>
-      </c>
-      <c r="N6" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="O6" s="3">
+      <c r="L6" s="3">
+        <v>0</v>
+      </c>
+      <c r="M6" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="N6" s="3">
+        <v>0</v>
+      </c>
+      <c r="O6" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="P6" s="3">
         <v>5</v>
       </c>
-      <c r="P6" s="3">
+      <c r="Q6" s="3">
         <v>35</v>
       </c>
-      <c r="Q6" s="3">
+      <c r="R6" s="3">
         <v>0.3</v>
       </c>
-      <c r="R6" s="3">
+      <c r="S6" s="3">
         <v>2.5</v>
       </c>
-      <c r="S6" s="3">
-        <v>1</v>
-      </c>
       <c r="T6" s="3">
+        <v>1</v>
+      </c>
+      <c r="U6" s="3">
         <v>0.5</v>
       </c>
     </row>
-    <row r="7" spans="1:20" s="3" customFormat="1" ht="49.5">
+    <row r="7" spans="1:21" s="3" customFormat="1" ht="49.5">
       <c r="A7" s="3">
         <v>10003002</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="G7" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="G7" s="3">
+      <c r="H7" s="3">
         <v>275</v>
       </c>
-      <c r="H7" s="3">
+      <c r="I7" s="3">
         <v>10</v>
       </c>
-      <c r="I7" s="3">
-        <v>0</v>
-      </c>
       <c r="J7" s="3">
         <v>0</v>
       </c>
       <c r="K7" s="3">
         <v>0</v>
       </c>
-      <c r="L7" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="M7" s="3">
-        <v>0</v>
-      </c>
-      <c r="N7" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="O7" s="3">
+      <c r="L7" s="3">
+        <v>0</v>
+      </c>
+      <c r="M7" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="N7" s="3">
+        <v>0</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="P7" s="3">
         <v>2</v>
       </c>
-      <c r="P7" s="3">
+      <c r="Q7" s="3">
         <v>25</v>
       </c>
-      <c r="Q7" s="3">
+      <c r="R7" s="3">
         <v>0.05</v>
       </c>
-      <c r="R7" s="3">
+      <c r="S7" s="3">
         <v>5</v>
       </c>
-      <c r="S7" s="3">
-        <v>1</v>
-      </c>
       <c r="T7" s="3">
+        <v>1</v>
+      </c>
+      <c r="U7" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:20" s="3" customFormat="1" ht="49.5">
+    <row r="8" spans="1:21" s="3" customFormat="1" ht="49.5">
       <c r="A8" s="3">
         <v>10003003</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D8" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H8" s="3">
+        <v>275</v>
+      </c>
+      <c r="I8" s="3">
+        <v>10</v>
+      </c>
+      <c r="J8" s="3">
+        <v>0</v>
+      </c>
+      <c r="K8" s="3">
+        <v>0</v>
+      </c>
+      <c r="L8" s="3">
+        <v>0</v>
+      </c>
+      <c r="M8" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="N8" s="3">
+        <v>0</v>
+      </c>
+      <c r="O8" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="E8" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="G8" s="3">
-        <v>275</v>
-      </c>
-      <c r="H8" s="3">
-        <v>10</v>
-      </c>
-      <c r="I8" s="3">
-        <v>0</v>
-      </c>
-      <c r="J8" s="3">
-        <v>0</v>
-      </c>
-      <c r="K8" s="3">
-        <v>0</v>
-      </c>
-      <c r="L8" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="M8" s="3">
-        <v>0</v>
-      </c>
-      <c r="N8" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="O8" s="3">
+      <c r="P8" s="3">
         <v>2</v>
       </c>
-      <c r="P8" s="3">
-        <v>0</v>
-      </c>
       <c r="Q8" s="3">
+        <v>0</v>
+      </c>
+      <c r="R8" s="3">
         <v>2</v>
       </c>
-      <c r="R8" s="3">
+      <c r="S8" s="3">
         <v>3</v>
       </c>
-      <c r="S8" s="3">
-        <v>1</v>
-      </c>
       <c r="T8" s="3">
+        <v>1</v>
+      </c>
+      <c r="U8" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:20" s="3" customFormat="1" ht="33">
+    <row r="9" spans="1:21" s="3" customFormat="1" ht="33">
       <c r="A9" s="3">
         <v>10003004</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="G9" s="3">
+        <v>58</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H9" s="3">
         <v>275</v>
       </c>
-      <c r="H9" s="3">
+      <c r="I9" s="3">
         <v>10</v>
       </c>
-      <c r="I9" s="3">
-        <v>0</v>
-      </c>
       <c r="J9" s="3">
         <v>0</v>
       </c>
       <c r="K9" s="3">
         <v>0</v>
       </c>
-      <c r="L9" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="M9" s="3">
-        <v>0</v>
-      </c>
-      <c r="N9" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="O9" s="3">
+      <c r="L9" s="3">
+        <v>0</v>
+      </c>
+      <c r="M9" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="N9" s="3">
+        <v>0</v>
+      </c>
+      <c r="O9" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="P9" s="3">
         <v>50</v>
       </c>
-      <c r="P9" s="3">
+      <c r="Q9" s="3">
         <v>25</v>
       </c>
-      <c r="Q9" s="3">
+      <c r="R9" s="3">
         <v>2</v>
       </c>
-      <c r="R9" s="3">
+      <c r="S9" s="3">
         <v>5</v>
       </c>
-      <c r="S9" s="3">
-        <v>1</v>
-      </c>
       <c r="T9" s="3">
+        <v>1</v>
+      </c>
+      <c r="U9" s="3">
         <v>0.2</v>
       </c>
     </row>
-    <row r="10" spans="1:20" s="3" customFormat="1">
+    <row r="10" spans="1:21" s="3" customFormat="1">
       <c r="A10" s="3">
         <v>10004001</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>29</v>
+        <v>65</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="G10" s="3">
+        <v>30</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H10" s="3">
         <v>120</v>
       </c>
-      <c r="H10" s="3">
+      <c r="I10" s="3">
         <v>5</v>
       </c>
-      <c r="I10" s="3">
-        <v>0</v>
-      </c>
       <c r="J10" s="3">
         <v>0</v>
       </c>
       <c r="K10" s="3">
         <v>0</v>
       </c>
-      <c r="L10" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="M10" s="3">
-        <v>0</v>
-      </c>
-      <c r="N10" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="O10" s="3">
+      <c r="L10" s="3">
+        <v>0</v>
+      </c>
+      <c r="M10" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="N10" s="3">
+        <v>0</v>
+      </c>
+      <c r="O10" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="P10" s="3">
         <v>5</v>
       </c>
-      <c r="P10" s="3">
+      <c r="Q10" s="3">
         <v>15</v>
       </c>
-      <c r="Q10" s="3">
+      <c r="R10" s="3">
         <v>0.05</v>
-      </c>
-      <c r="R10" s="3">
-        <v>5</v>
       </c>
       <c r="S10" s="3">
         <v>5</v>
       </c>
       <c r="T10" s="3">
+        <v>5</v>
+      </c>
+      <c r="U10" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:20" s="3" customFormat="1">
+    <row r="11" spans="1:21" s="3" customFormat="1">
       <c r="A11" s="3">
         <v>10004002</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>29</v>
+        <v>65</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="G11" s="3">
+        <v>30</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H11" s="3">
         <v>200</v>
       </c>
-      <c r="H11" s="3">
+      <c r="I11" s="3">
         <v>5</v>
       </c>
-      <c r="I11" s="3">
-        <v>0</v>
-      </c>
       <c r="J11" s="3">
         <v>0</v>
       </c>
       <c r="K11" s="3">
         <v>0</v>
       </c>
-      <c r="L11" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="M11" s="3">
-        <v>0</v>
-      </c>
-      <c r="N11" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="O11" s="3">
-        <v>1</v>
+      <c r="L11" s="3">
+        <v>0</v>
+      </c>
+      <c r="M11" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="N11" s="3">
+        <v>0</v>
+      </c>
+      <c r="O11" s="3" t="s">
+        <v>51</v>
       </c>
       <c r="P11" s="3">
         <v>1</v>
@@ -1365,12 +1395,15 @@
       <c r="T11" s="3">
         <v>1</v>
       </c>
+      <c r="U11" s="3">
+        <v>1</v>
+      </c>
     </row>
-    <row r="12" spans="1:20" s="3" customFormat="1"/>
-    <row r="13" spans="1:20" s="3" customFormat="1"/>
-    <row r="14" spans="1:20" s="3" customFormat="1"/>
-    <row r="15" spans="1:20" s="3" customFormat="1"/>
-    <row r="16" spans="1:20" s="3" customFormat="1"/>
+    <row r="12" spans="1:21" s="3" customFormat="1"/>
+    <row r="13" spans="1:21" s="3" customFormat="1"/>
+    <row r="14" spans="1:21" s="3" customFormat="1"/>
+    <row r="15" spans="1:21" s="3" customFormat="1"/>
+    <row r="16" spans="1:21" s="3" customFormat="1"/>
     <row r="17" s="3" customFormat="1"/>
     <row r="18" s="3" customFormat="1"/>
     <row r="19" s="3" customFormat="1"/>

</xml_diff>

<commit_message>
Remove: 불필요 스크립트 삭제(Player SO)
</commit_message>
<xml_diff>
--- a/Assets/@Project/Scripts/Data/RawData/PartDbSheet.xlsx
+++ b/Assets/@Project/Scripts/Data/RawData/PartDbSheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27528"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{478779E2-8A92-45C0-B4FD-8637983234A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8C69F15E-8619-4BC9-95E3-503D5021272F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="72">
   <si>
     <t>dev_ID</t>
   </si>
@@ -94,6 +94,9 @@
   </si>
   <si>
     <t>shotErrorRange</t>
+  </si>
+  <si>
+    <t>ammo</t>
   </si>
   <si>
     <t>Lower_01</t>
@@ -235,6 +238,9 @@
   </si>
   <si>
     <t>Prefabs/Parts/Weapon_Shoulder/Weapon_Shoulder_01</t>
+  </si>
+  <si>
+    <t>Images/Weapon_S01</t>
   </si>
   <si>
     <t>TEST WEAPON_SHOULDER</t>
@@ -675,10 +681,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U22"/>
+  <dimension ref="A1:V22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="V11" sqref="V11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -700,7 +706,7 @@
     <col min="21" max="21" width="15.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="1" customFormat="1">
+    <row r="1" spans="1:22" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -764,26 +770,29 @@
       <c r="U1" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="2" spans="1:21" s="2" customFormat="1" ht="33">
+    <row r="2" spans="1:22" s="2" customFormat="1" ht="33">
       <c r="A2" s="2">
         <v>10001001</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H2" s="2">
         <v>2300</v>
@@ -807,7 +816,7 @@
         <v>0</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="P2" s="2">
         <v>0</v>
@@ -827,25 +836,28 @@
       <c r="U2" s="2">
         <v>0</v>
       </c>
+      <c r="V2" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:21" s="2" customFormat="1">
+    <row r="3" spans="1:22" s="2" customFormat="1">
       <c r="A3" s="2">
         <v>10001002</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H3" s="2">
         <v>10000</v>
@@ -869,7 +881,7 @@
         <v>0</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="P3" s="2">
         <v>0</v>
@@ -889,26 +901,29 @@
       <c r="U3" s="2">
         <v>0</v>
       </c>
+      <c r="V3" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:21" s="2" customFormat="1" ht="49.5">
+    <row r="4" spans="1:22" s="2" customFormat="1" ht="49.5">
       <c r="A4" s="2">
         <v>10002001</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H4" s="2">
         <v>3000</v>
@@ -932,7 +947,7 @@
         <v>3</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="P4" s="2">
         <v>0</v>
@@ -952,25 +967,28 @@
       <c r="U4" s="2">
         <v>0</v>
       </c>
+      <c r="V4" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:21" s="2" customFormat="1">
+    <row r="5" spans="1:22" s="2" customFormat="1">
       <c r="A5" s="2">
         <v>10002002</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>35</v>
       </c>
       <c r="H5" s="2">
         <v>10000</v>
@@ -994,7 +1012,7 @@
         <v>1000</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="P5" s="2">
         <v>0</v>
@@ -1014,28 +1032,31 @@
       <c r="U5" s="2">
         <v>0</v>
       </c>
+      <c r="V5" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:21" s="3" customFormat="1" ht="33">
+    <row r="6" spans="1:22" s="3" customFormat="1" ht="33">
       <c r="A6" s="3">
         <v>10003001</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H6" s="3">
         <v>350</v>
@@ -1059,7 +1080,7 @@
         <v>0</v>
       </c>
       <c r="O6" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="P6" s="3">
         <v>5</v>
@@ -1079,28 +1100,31 @@
       <c r="U6" s="3">
         <v>0.5</v>
       </c>
+      <c r="V6" s="3">
+        <v>50</v>
+      </c>
     </row>
-    <row r="7" spans="1:21" s="3" customFormat="1" ht="49.5">
+    <row r="7" spans="1:22" s="3" customFormat="1" ht="49.5">
       <c r="A7" s="3">
         <v>10003002</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H7" s="3">
         <v>275</v>
@@ -1124,7 +1148,7 @@
         <v>0</v>
       </c>
       <c r="O7" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="P7" s="3">
         <v>2</v>
@@ -1144,28 +1168,31 @@
       <c r="U7" s="3">
         <v>2</v>
       </c>
+      <c r="V7" s="3">
+        <v>200</v>
+      </c>
     </row>
-    <row r="8" spans="1:21" s="3" customFormat="1" ht="49.5">
+    <row r="8" spans="1:22" s="3" customFormat="1" ht="49.5">
       <c r="A8" s="3">
         <v>10003003</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H8" s="3">
         <v>275</v>
@@ -1189,7 +1216,7 @@
         <v>0</v>
       </c>
       <c r="O8" s="3" t="s">
-        <v>51</v>
+        <v>27</v>
       </c>
       <c r="P8" s="3">
         <v>2</v>
@@ -1209,28 +1236,31 @@
       <c r="U8" s="3">
         <v>0</v>
       </c>
+      <c r="V8" s="3">
+        <v>1</v>
+      </c>
     </row>
-    <row r="9" spans="1:21" s="3" customFormat="1" ht="33">
+    <row r="9" spans="1:22" s="3" customFormat="1" ht="33">
       <c r="A9" s="3">
         <v>10003004</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H9" s="3">
         <v>275</v>
@@ -1254,7 +1284,7 @@
         <v>0</v>
       </c>
       <c r="O9" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="P9" s="3">
         <v>50</v>
@@ -1274,25 +1304,31 @@
       <c r="U9" s="3">
         <v>0.2</v>
       </c>
+      <c r="V9" s="3">
+        <v>10</v>
+      </c>
     </row>
-    <row r="10" spans="1:21" s="3" customFormat="1">
+    <row r="10" spans="1:22" s="3" customFormat="1">
       <c r="A10" s="3">
         <v>10004001</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>66</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="H10" s="3">
         <v>120</v>
@@ -1316,7 +1352,7 @@
         <v>0</v>
       </c>
       <c r="O10" s="3" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="P10" s="3">
         <v>5</v>
@@ -1336,25 +1372,28 @@
       <c r="U10" s="3">
         <v>1</v>
       </c>
+      <c r="V10" s="3">
+        <v>80</v>
+      </c>
     </row>
-    <row r="11" spans="1:21" s="3" customFormat="1">
+    <row r="11" spans="1:22" s="3" customFormat="1">
       <c r="A11" s="3">
         <v>10004002</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G11" s="3" t="s">
         <v>68</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>66</v>
       </c>
       <c r="H11" s="3">
         <v>200</v>
@@ -1378,7 +1417,7 @@
         <v>0</v>
       </c>
       <c r="O11" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="P11" s="3">
         <v>1</v>
@@ -1398,12 +1437,15 @@
       <c r="U11" s="3">
         <v>1</v>
       </c>
+      <c r="V11" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="12" spans="1:21" s="3" customFormat="1"/>
-    <row r="13" spans="1:21" s="3" customFormat="1"/>
-    <row r="14" spans="1:21" s="3" customFormat="1"/>
-    <row r="15" spans="1:21" s="3" customFormat="1"/>
-    <row r="16" spans="1:21" s="3" customFormat="1"/>
+    <row r="12" spans="1:22" s="3" customFormat="1"/>
+    <row r="13" spans="1:22" s="3" customFormat="1"/>
+    <row r="14" spans="1:22" s="3" customFormat="1"/>
+    <row r="15" spans="1:22" s="3" customFormat="1"/>
+    <row r="16" spans="1:22" s="3" customFormat="1"/>
     <row r="17" s="3" customFormat="1"/>
     <row r="18" s="3" customFormat="1"/>
     <row r="19" s="3" customFormat="1"/>

</xml_diff>

<commit_message>
Refactor: PartChangeBtn 코드 개선 및 파츠 이미지 추가
</commit_message>
<xml_diff>
--- a/Assets/@Project/Scripts/Data/RawData/PartDbSheet.xlsx
+++ b/Assets/@Project/Scripts/Data/RawData/PartDbSheet.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27528"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27601"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5D16D0FE-87CC-46AF-B97F-90F10BED220F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{45401EA0-4F07-44B1-9C23-BE5040374B90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="73">
   <si>
     <t>dev_ID</t>
   </si>
@@ -103,6 +103,9 @@
   </si>
   <si>
     <t>Prefabs/Parts/Lower/Lower_01</t>
+  </si>
+  <si>
+    <t>Images/Lower_01</t>
   </si>
   <si>
     <t>DG-001</t>
@@ -121,6 +124,9 @@
     <t>Prefabs/Parts/Lower/Lower_02Temp</t>
   </si>
   <si>
+    <t>Images/Lower_02</t>
+  </si>
+  <si>
     <t>TEST LEG</t>
   </si>
   <si>
@@ -131,6 +137,9 @@
   </si>
   <si>
     <t>Prefabs/Parts/Upper/Upper_01</t>
+  </si>
+  <si>
+    <t>Images/Upper_01</t>
   </si>
   <si>
     <t>UH-001</t>
@@ -147,6 +156,9 @@
     <t>Prefabs/Parts/Upper/Upper_02Temp</t>
   </si>
   <si>
+    <t>Images/Upper_02</t>
+  </si>
+  <si>
     <t>TEST HEAD</t>
   </si>
   <si>
@@ -156,7 +168,7 @@
     <t>Prefabs/Parts/Weapon_Arm/Weapon_Arm_01</t>
   </si>
   <si>
-    <t>Images/Weapon_01</t>
+    <t>Images/Weapon_A01</t>
   </si>
   <si>
     <t>CA-STD</t>
@@ -175,7 +187,7 @@
     <t>Prefabs/Parts/Weapon_Arm/Weapon_Arm_02</t>
   </si>
   <si>
-    <t>Images/Weapon_02</t>
+    <t>Images/Weapon_A02</t>
   </si>
   <si>
     <t>GA-S</t>
@@ -195,7 +207,7 @@
     <t>Prefabs/Parts/Weapon_Arm/Weapon_Arm_03</t>
   </si>
   <si>
-    <t>Images/Weapon_03</t>
+    <t>Images/Weapon_A03</t>
   </si>
   <si>
     <t>LC-S</t>
@@ -212,7 +224,7 @@
     <t>Prefabs/Parts/Weapon_Arm/Weapon_Arm_04</t>
   </si>
   <si>
-    <t>Images/Weapon_04</t>
+    <t>Images/Weapon_A04</t>
   </si>
   <si>
     <t>CA-AP</t>
@@ -244,6 +256,9 @@
   </si>
   <si>
     <t>Prefabs/Parts/Weapon_Shoulder/Weapon_Shoulder_02</t>
+  </si>
+  <si>
+    <t>Images/Weapon_S02</t>
   </si>
 </sst>
 </file>
@@ -671,8 +686,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="W13" sqref="W13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -772,12 +787,14 @@
       <c r="C2" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="5"/>
+      <c r="D2" s="5" t="s">
+        <v>24</v>
+      </c>
       <c r="E2" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G2" s="2">
         <v>2300</v>
@@ -801,7 +818,7 @@
         <v>0</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O2" s="2">
         <v>0</v>
@@ -833,16 +850,19 @@
         <v>10001002</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G3" s="2">
         <v>10000</v>
@@ -866,7 +886,7 @@
         <v>0</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O3" s="2">
         <v>0</v>
@@ -898,17 +918,19 @@
         <v>10002001</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D4" s="5"/>
+        <v>34</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>35</v>
+      </c>
       <c r="E4" s="2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="G4" s="2">
         <v>3000</v>
@@ -932,7 +954,7 @@
         <v>3</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O4" s="2">
         <v>0</v>
@@ -964,16 +986,19 @@
         <v>10002002</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>40</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G5" s="2">
         <v>10000</v>
@@ -997,7 +1022,7 @@
         <v>1000</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O5" s="2">
         <v>0</v>
@@ -1029,19 +1054,19 @@
         <v>10003001</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="G6" s="3">
         <v>350</v>
@@ -1065,7 +1090,7 @@
         <v>0</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="O6" s="3">
         <v>5</v>
@@ -1097,19 +1122,19 @@
         <v>10003002</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="G7" s="3">
         <v>275</v>
@@ -1133,7 +1158,7 @@
         <v>0</v>
       </c>
       <c r="N7" s="3" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="O7" s="3">
         <v>2</v>
@@ -1165,19 +1190,19 @@
         <v>10003003</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="G8" s="3">
         <v>275</v>
@@ -1201,7 +1226,7 @@
         <v>0</v>
       </c>
       <c r="N8" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O8" s="3">
         <v>2</v>
@@ -1233,19 +1258,19 @@
         <v>10003004</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="G9" s="3">
         <v>275</v>
@@ -1269,7 +1294,7 @@
         <v>0</v>
       </c>
       <c r="N9" s="3" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="O9" s="3">
         <v>50</v>
@@ -1301,19 +1326,19 @@
         <v>10004001</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G10" s="3">
         <v>120</v>
@@ -1337,7 +1362,7 @@
         <v>0</v>
       </c>
       <c r="N10" s="3" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="O10" s="3">
         <v>5</v>
@@ -1369,16 +1394,19 @@
         <v>10004002</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>67</v>
+        <v>71</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>72</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G11" s="3">
         <v>200</v>
@@ -1402,7 +1430,7 @@
         <v>0</v>
       </c>
       <c r="N11" s="3" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="O11" s="3">
         <v>1</v>

</xml_diff>

<commit_message>
Feat: Player HoverState 추가 및 State 로직 수정
</commit_message>
<xml_diff>
--- a/Assets/@Project/Scripts/Data/RawData/PartDbSheet.xlsx
+++ b/Assets/@Project/Scripts/Data/RawData/PartDbSheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27601"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0B8C6AED-5001-4269-938C-3599D6175630}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7EA9EB36-C93D-4582-B44E-52A5E23E9EF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="85">
   <si>
     <t>dev_ID</t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t>smoothRotation</t>
+  </si>
+  <si>
+    <t>hovering</t>
   </si>
   <si>
     <t>bulletPrefab_Path</t>
@@ -722,10 +725,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W22"/>
+  <dimension ref="A1:X22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="U14" sqref="U14"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -738,16 +741,16 @@
     <col min="6" max="6" width="47.875" customWidth="1"/>
     <col min="10" max="10" width="13.125" customWidth="1"/>
     <col min="11" max="11" width="13" customWidth="1"/>
-    <col min="13" max="13" width="16.375" customWidth="1"/>
-    <col min="14" max="14" width="46.25" customWidth="1"/>
-    <col min="16" max="16" width="14.5" customWidth="1"/>
-    <col min="18" max="18" width="14.625" customWidth="1"/>
-    <col min="19" max="19" width="18.5" customWidth="1"/>
-    <col min="20" max="20" width="15.125" customWidth="1"/>
-    <col min="22" max="22" width="14.875" customWidth="1"/>
+    <col min="13" max="14" width="16.375" customWidth="1"/>
+    <col min="15" max="15" width="46.25" customWidth="1"/>
+    <col min="17" max="17" width="14.5" customWidth="1"/>
+    <col min="19" max="19" width="14.625" customWidth="1"/>
+    <col min="20" max="20" width="18.5" customWidth="1"/>
+    <col min="21" max="21" width="15.125" customWidth="1"/>
+    <col min="23" max="23" width="14.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="1" customFormat="1">
+    <row r="1" spans="1:24" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -817,25 +820,28 @@
       <c r="W1" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="X1" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="2" spans="1:23" s="2" customFormat="1" ht="33">
+    <row r="2" spans="1:24" s="2" customFormat="1" ht="33">
       <c r="A2" s="2">
         <v>10001001</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G2" s="2">
         <v>2300</v>
@@ -858,11 +864,11 @@
       <c r="M2" s="2">
         <v>0</v>
       </c>
-      <c r="N2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="O2" s="2">
-        <v>0</v>
+      <c r="N2" s="2">
+        <v>0</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="P2" s="2">
         <v>0</v>
@@ -882,31 +888,34 @@
       <c r="U2" s="2">
         <v>0</v>
       </c>
-      <c r="V2" s="2" t="b">
+      <c r="V2" s="2">
         <v>0</v>
       </c>
       <c r="W2" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="X2" s="2" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:23" s="2" customFormat="1">
+    <row r="3" spans="1:24" s="2" customFormat="1">
       <c r="A3" s="2">
         <v>10001002</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G3" s="2">
         <v>10000</v>
@@ -929,11 +938,11 @@
       <c r="M3" s="2">
         <v>0</v>
       </c>
-      <c r="N3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="O3" s="2">
-        <v>0</v>
+      <c r="N3" s="2">
+        <v>0</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="P3" s="2">
         <v>0</v>
@@ -953,31 +962,34 @@
       <c r="U3" s="2">
         <v>0</v>
       </c>
-      <c r="V3" s="2" t="b">
+      <c r="V3" s="2">
         <v>0</v>
       </c>
       <c r="W3" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="X3" s="2" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:23" s="2" customFormat="1" ht="49.5">
+    <row r="4" spans="1:24" s="2" customFormat="1" ht="49.5">
       <c r="A4" s="2">
         <v>10002001</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G4" s="2">
         <v>3000</v>
@@ -1000,11 +1012,11 @@
       <c r="M4" s="2">
         <v>3</v>
       </c>
-      <c r="N4" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="O4" s="2">
-        <v>0</v>
+      <c r="N4" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="P4" s="2">
         <v>0</v>
@@ -1024,31 +1036,34 @@
       <c r="U4" s="2">
         <v>0</v>
       </c>
-      <c r="V4" s="2" t="b">
+      <c r="V4" s="2">
         <v>0</v>
       </c>
       <c r="W4" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="X4" s="2" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:23" s="2" customFormat="1">
+    <row r="5" spans="1:24" s="2" customFormat="1">
       <c r="A5" s="2">
         <v>10002002</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G5" s="2">
         <v>10000</v>
@@ -1071,11 +1086,11 @@
       <c r="M5" s="2">
         <v>1000</v>
       </c>
-      <c r="N5" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="O5" s="2">
-        <v>0</v>
+      <c r="N5" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="P5" s="2">
         <v>0</v>
@@ -1095,31 +1110,34 @@
       <c r="U5" s="2">
         <v>0</v>
       </c>
-      <c r="V5" s="2" t="b">
+      <c r="V5" s="2">
         <v>0</v>
       </c>
       <c r="W5" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="X5" s="2" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:23" s="3" customFormat="1" ht="33">
+    <row r="6" spans="1:24" s="3" customFormat="1" ht="33">
       <c r="A6" s="3">
         <v>10003001</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G6" s="3">
         <v>350</v>
@@ -1142,55 +1160,58 @@
       <c r="M6" s="3">
         <v>0</v>
       </c>
-      <c r="N6" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="O6" s="3">
+      <c r="N6" s="3">
+        <v>0</v>
+      </c>
+      <c r="O6" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="P6" s="3">
         <v>5</v>
       </c>
-      <c r="P6" s="3">
+      <c r="Q6" s="3">
         <v>25</v>
       </c>
-      <c r="Q6" s="3">
+      <c r="R6" s="3">
         <v>0.3</v>
       </c>
-      <c r="R6" s="3">
+      <c r="S6" s="3">
         <v>2.5</v>
       </c>
-      <c r="S6" s="3">
-        <v>1</v>
-      </c>
       <c r="T6" s="3">
+        <v>1</v>
+      </c>
+      <c r="U6" s="3">
         <v>0.5</v>
       </c>
-      <c r="U6" s="3">
+      <c r="V6" s="3">
         <v>50</v>
       </c>
-      <c r="V6" s="3" t="b">
-        <v>1</v>
-      </c>
       <c r="W6" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="X6" s="3" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:23" s="3" customFormat="1" ht="49.5">
+    <row r="7" spans="1:24" s="3" customFormat="1" ht="49.5">
       <c r="A7" s="3">
         <v>10003002</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G7" s="3">
         <v>275</v>
@@ -1213,55 +1234,58 @@
       <c r="M7" s="3">
         <v>0</v>
       </c>
-      <c r="N7" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="O7" s="3">
+      <c r="N7" s="3">
+        <v>0</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="P7" s="3">
         <v>2</v>
       </c>
-      <c r="P7" s="3">
+      <c r="Q7" s="3">
         <v>35</v>
       </c>
-      <c r="Q7" s="3">
+      <c r="R7" s="3">
         <v>0.05</v>
       </c>
-      <c r="R7" s="3">
+      <c r="S7" s="3">
         <v>5</v>
       </c>
-      <c r="S7" s="3">
-        <v>1</v>
-      </c>
       <c r="T7" s="3">
+        <v>1</v>
+      </c>
+      <c r="U7" s="3">
         <v>2</v>
       </c>
-      <c r="U7" s="3">
+      <c r="V7" s="3">
         <v>200</v>
       </c>
-      <c r="V7" s="3" t="b">
-        <v>1</v>
-      </c>
       <c r="W7" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="X7" s="3" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:23" s="3" customFormat="1" ht="49.5">
+    <row r="8" spans="1:24" s="3" customFormat="1" ht="49.5">
       <c r="A8" s="3">
         <v>10003003</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G8" s="3">
         <v>275</v>
@@ -1284,55 +1308,58 @@
       <c r="M8" s="3">
         <v>0</v>
       </c>
-      <c r="N8" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="O8" s="3">
+      <c r="N8" s="3">
+        <v>0</v>
+      </c>
+      <c r="O8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="P8" s="3">
         <v>2</v>
       </c>
-      <c r="P8" s="3">
-        <v>0</v>
-      </c>
       <c r="Q8" s="3">
+        <v>0</v>
+      </c>
+      <c r="R8" s="3">
         <v>2</v>
       </c>
-      <c r="R8" s="3">
+      <c r="S8" s="3">
         <v>3</v>
       </c>
-      <c r="S8" s="3">
-        <v>1</v>
-      </c>
       <c r="T8" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U8" s="3">
-        <v>1</v>
-      </c>
-      <c r="V8" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="V8" s="3">
         <v>1</v>
       </c>
       <c r="W8" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="X8" s="3" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:23" s="3" customFormat="1" ht="33">
+    <row r="9" spans="1:24" s="3" customFormat="1" ht="33">
       <c r="A9" s="3">
         <v>10003004</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G9" s="3">
         <v>275</v>
@@ -1355,55 +1382,58 @@
       <c r="M9" s="3">
         <v>0</v>
       </c>
-      <c r="N9" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="O9" s="3">
+      <c r="N9" s="3">
+        <v>0</v>
+      </c>
+      <c r="O9" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="P9" s="3">
         <v>50</v>
       </c>
-      <c r="P9" s="3">
+      <c r="Q9" s="3">
         <v>25</v>
       </c>
-      <c r="Q9" s="3">
+      <c r="R9" s="3">
         <v>2</v>
       </c>
-      <c r="R9" s="3">
+      <c r="S9" s="3">
         <v>5</v>
       </c>
-      <c r="S9" s="3">
-        <v>1</v>
-      </c>
       <c r="T9" s="3">
+        <v>1</v>
+      </c>
+      <c r="U9" s="3">
         <v>0.2</v>
       </c>
-      <c r="U9" s="3">
+      <c r="V9" s="3">
         <v>10</v>
       </c>
-      <c r="V9" s="3" t="b">
-        <v>1</v>
-      </c>
       <c r="W9" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="X9" s="3" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:23" s="3" customFormat="1" ht="33">
+    <row r="10" spans="1:24" s="3" customFormat="1" ht="33">
       <c r="A10" s="3">
         <v>10004001</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G10" s="3">
         <v>120</v>
@@ -1426,55 +1456,58 @@
       <c r="M10" s="3">
         <v>0</v>
       </c>
-      <c r="N10" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="O10" s="3">
+      <c r="N10" s="3">
+        <v>0</v>
+      </c>
+      <c r="O10" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="P10" s="3">
         <v>5</v>
       </c>
-      <c r="P10" s="3">
+      <c r="Q10" s="3">
         <v>15</v>
       </c>
-      <c r="Q10" s="3">
+      <c r="R10" s="3">
         <v>0.05</v>
-      </c>
-      <c r="R10" s="3">
-        <v>5</v>
       </c>
       <c r="S10" s="3">
         <v>5</v>
       </c>
       <c r="T10" s="3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="U10" s="3">
+        <v>1</v>
+      </c>
+      <c r="V10" s="3">
         <v>10</v>
       </c>
-      <c r="V10" s="3" t="b">
-        <v>0</v>
-      </c>
       <c r="W10" s="3" t="b">
         <v>0</v>
       </c>
+      <c r="X10" s="3" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="11" spans="1:23" s="3" customFormat="1" ht="49.5">
+    <row r="11" spans="1:24" s="3" customFormat="1" ht="49.5">
       <c r="A11" s="3">
         <v>10004002</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G11" s="3">
         <v>200</v>
@@ -1497,55 +1530,58 @@
       <c r="M11" s="3">
         <v>0</v>
       </c>
-      <c r="N11" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="O11" s="3">
+      <c r="N11" s="3">
+        <v>0</v>
+      </c>
+      <c r="O11" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="P11" s="3">
         <v>50</v>
       </c>
-      <c r="P11" s="3">
+      <c r="Q11" s="3">
         <v>20</v>
       </c>
-      <c r="Q11" s="3">
+      <c r="R11" s="3">
         <v>0.5</v>
       </c>
-      <c r="R11" s="3">
+      <c r="S11" s="3">
         <v>5</v>
       </c>
-      <c r="S11" s="3">
-        <v>1</v>
-      </c>
       <c r="T11" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U11" s="3">
+        <v>0</v>
+      </c>
+      <c r="V11" s="3">
         <v>10</v>
       </c>
-      <c r="V11" s="3" t="b">
-        <v>0</v>
-      </c>
       <c r="W11" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="X11" s="3" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:23" s="3" customFormat="1" ht="49.5">
+    <row r="12" spans="1:24" s="3" customFormat="1" ht="49.5">
       <c r="A12" s="3">
         <v>10004003</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="G12" s="3">
         <v>150</v>
@@ -1568,41 +1604,44 @@
       <c r="M12" s="3">
         <v>0</v>
       </c>
-      <c r="N12" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="O12" s="3">
+      <c r="N12" s="3">
+        <v>0</v>
+      </c>
+      <c r="O12" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="P12" s="3">
         <v>125</v>
       </c>
-      <c r="P12" s="3">
+      <c r="Q12" s="3">
         <v>50</v>
       </c>
-      <c r="Q12" s="3">
-        <v>0</v>
-      </c>
       <c r="R12" s="3">
+        <v>0</v>
+      </c>
+      <c r="S12" s="3">
         <v>3</v>
       </c>
-      <c r="S12" s="3">
-        <v>1</v>
-      </c>
       <c r="T12" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U12" s="3">
+        <v>0</v>
+      </c>
+      <c r="V12" s="3">
         <v>10</v>
       </c>
-      <c r="V12" s="3" t="b">
-        <v>0</v>
-      </c>
       <c r="W12" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="X12" s="3" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:23" s="3" customFormat="1"/>
-    <row r="14" spans="1:23" s="3" customFormat="1"/>
-    <row r="15" spans="1:23" s="3" customFormat="1"/>
-    <row r="16" spans="1:23" s="3" customFormat="1"/>
+    <row r="13" spans="1:24" s="3" customFormat="1"/>
+    <row r="14" spans="1:24" s="3" customFormat="1"/>
+    <row r="15" spans="1:24" s="3" customFormat="1"/>
+    <row r="16" spans="1:24" s="3" customFormat="1"/>
     <row r="17" s="3" customFormat="1"/>
     <row r="18" s="3" customFormat="1"/>
     <row r="19" s="3" customFormat="1"/>

</xml_diff>

<commit_message>
Feat: Player 조작감 개선
</commit_message>
<xml_diff>
--- a/Assets/@Project/Scripts/Data/RawData/PartDbSheet.xlsx
+++ b/Assets/@Project/Scripts/Data/RawData/PartDbSheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27601"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7EA9EB36-C93D-4582-B44E-52A5E23E9EF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{67E7B5E7-E3F9-418A-B837-B648D20726CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="86">
   <si>
     <t>dev_ID</t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t>smoothRotation</t>
+  </si>
+  <si>
+    <t>boosterGauge</t>
   </si>
   <si>
     <t>hovering</t>
@@ -725,10 +728,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X22"/>
+  <dimension ref="A1:Y22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -741,16 +744,16 @@
     <col min="6" max="6" width="47.875" customWidth="1"/>
     <col min="10" max="10" width="13.125" customWidth="1"/>
     <col min="11" max="11" width="13" customWidth="1"/>
-    <col min="13" max="14" width="16.375" customWidth="1"/>
-    <col min="15" max="15" width="46.25" customWidth="1"/>
-    <col min="17" max="17" width="14.5" customWidth="1"/>
-    <col min="19" max="19" width="14.625" customWidth="1"/>
-    <col min="20" max="20" width="18.5" customWidth="1"/>
-    <col min="21" max="21" width="15.125" customWidth="1"/>
-    <col min="23" max="23" width="14.875" customWidth="1"/>
+    <col min="13" max="15" width="16.375" customWidth="1"/>
+    <col min="16" max="16" width="46.25" customWidth="1"/>
+    <col min="18" max="18" width="14.5" customWidth="1"/>
+    <col min="20" max="20" width="14.625" customWidth="1"/>
+    <col min="21" max="21" width="18.5" customWidth="1"/>
+    <col min="22" max="22" width="15.125" customWidth="1"/>
+    <col min="24" max="24" width="14.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="1" customFormat="1">
+    <row r="1" spans="1:25" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -823,25 +826,28 @@
       <c r="X1" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="Y1" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="2" spans="1:24" s="2" customFormat="1" ht="33">
+    <row r="2" spans="1:25" s="2" customFormat="1" ht="33">
       <c r="A2" s="2">
         <v>10001001</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G2" s="2">
         <v>2300</v>
@@ -867,11 +873,11 @@
       <c r="N2" s="2">
         <v>0</v>
       </c>
-      <c r="O2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="P2" s="2">
-        <v>0</v>
+      <c r="O2" s="2">
+        <v>0</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="Q2" s="2">
         <v>0</v>
@@ -891,31 +897,34 @@
       <c r="V2" s="2">
         <v>0</v>
       </c>
-      <c r="W2" s="2" t="b">
+      <c r="W2" s="2">
         <v>0</v>
       </c>
       <c r="X2" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="Y2" s="2" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:24" s="2" customFormat="1">
+    <row r="3" spans="1:25" s="2" customFormat="1">
       <c r="A3" s="2">
         <v>10001002</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G3" s="2">
         <v>10000</v>
@@ -941,11 +950,11 @@
       <c r="N3" s="2">
         <v>0</v>
       </c>
-      <c r="O3" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="P3" s="2">
-        <v>0</v>
+      <c r="O3" s="2">
+        <v>0</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="Q3" s="2">
         <v>0</v>
@@ -965,31 +974,34 @@
       <c r="V3" s="2">
         <v>0</v>
       </c>
-      <c r="W3" s="2" t="b">
+      <c r="W3" s="2">
         <v>0</v>
       </c>
       <c r="X3" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="Y3" s="2" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:24" s="2" customFormat="1" ht="49.5">
+    <row r="4" spans="1:25" s="2" customFormat="1" ht="49.5">
       <c r="A4" s="2">
         <v>10002001</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G4" s="2">
         <v>3000</v>
@@ -1013,13 +1025,13 @@
         <v>3</v>
       </c>
       <c r="N4" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="P4" s="2">
-        <v>0</v>
+        <v>100</v>
+      </c>
+      <c r="O4" s="2">
+        <v>2</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="Q4" s="2">
         <v>0</v>
@@ -1039,31 +1051,34 @@
       <c r="V4" s="2">
         <v>0</v>
       </c>
-      <c r="W4" s="2" t="b">
+      <c r="W4" s="2">
         <v>0</v>
       </c>
       <c r="X4" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="Y4" s="2" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:24" s="2" customFormat="1">
+    <row r="5" spans="1:25" s="2" customFormat="1">
       <c r="A5" s="2">
         <v>10002002</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G5" s="2">
         <v>10000</v>
@@ -1087,13 +1102,13 @@
         <v>1000</v>
       </c>
       <c r="N5" s="2">
+        <v>120</v>
+      </c>
+      <c r="O5" s="2">
         <v>0.1</v>
       </c>
-      <c r="O5" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="P5" s="2">
-        <v>0</v>
+      <c r="P5" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="Q5" s="2">
         <v>0</v>
@@ -1113,31 +1128,34 @@
       <c r="V5" s="2">
         <v>0</v>
       </c>
-      <c r="W5" s="2" t="b">
+      <c r="W5" s="2">
         <v>0</v>
       </c>
       <c r="X5" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="Y5" s="2" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:24" s="3" customFormat="1" ht="33">
+    <row r="6" spans="1:25" s="3" customFormat="1" ht="33">
       <c r="A6" s="3">
         <v>10003001</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G6" s="3">
         <v>350</v>
@@ -1160,58 +1178,58 @@
       <c r="M6" s="3">
         <v>0</v>
       </c>
-      <c r="N6" s="3">
-        <v>0</v>
-      </c>
-      <c r="O6" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="P6" s="3">
+      <c r="O6" s="3">
+        <v>0</v>
+      </c>
+      <c r="P6" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q6" s="3">
         <v>5</v>
       </c>
-      <c r="Q6" s="3">
+      <c r="R6" s="3">
         <v>25</v>
       </c>
-      <c r="R6" s="3">
+      <c r="S6" s="3">
         <v>0.3</v>
       </c>
-      <c r="S6" s="3">
+      <c r="T6" s="3">
         <v>2.5</v>
       </c>
-      <c r="T6" s="3">
-        <v>1</v>
-      </c>
       <c r="U6" s="3">
+        <v>1</v>
+      </c>
+      <c r="V6" s="3">
         <v>0.5</v>
       </c>
-      <c r="V6" s="3">
+      <c r="W6" s="3">
         <v>50</v>
       </c>
-      <c r="W6" s="3" t="b">
-        <v>1</v>
-      </c>
       <c r="X6" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y6" s="3" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:24" s="3" customFormat="1" ht="49.5">
+    <row r="7" spans="1:25" s="3" customFormat="1" ht="49.5">
       <c r="A7" s="3">
         <v>10003002</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G7" s="3">
         <v>275</v>
@@ -1234,58 +1252,58 @@
       <c r="M7" s="3">
         <v>0</v>
       </c>
-      <c r="N7" s="3">
-        <v>0</v>
-      </c>
-      <c r="O7" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="P7" s="3">
+      <c r="O7" s="3">
+        <v>0</v>
+      </c>
+      <c r="P7" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q7" s="3">
         <v>2</v>
       </c>
-      <c r="Q7" s="3">
+      <c r="R7" s="3">
         <v>35</v>
       </c>
-      <c r="R7" s="3">
+      <c r="S7" s="3">
         <v>0.05</v>
       </c>
-      <c r="S7" s="3">
+      <c r="T7" s="3">
         <v>5</v>
       </c>
-      <c r="T7" s="3">
-        <v>1</v>
-      </c>
       <c r="U7" s="3">
+        <v>1</v>
+      </c>
+      <c r="V7" s="3">
         <v>2</v>
       </c>
-      <c r="V7" s="3">
+      <c r="W7" s="3">
         <v>200</v>
       </c>
-      <c r="W7" s="3" t="b">
-        <v>1</v>
-      </c>
       <c r="X7" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y7" s="3" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:24" s="3" customFormat="1" ht="49.5">
+    <row r="8" spans="1:25" s="3" customFormat="1" ht="49.5">
       <c r="A8" s="3">
         <v>10003003</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G8" s="3">
         <v>275</v>
@@ -1308,58 +1326,58 @@
       <c r="M8" s="3">
         <v>0</v>
       </c>
-      <c r="N8" s="3">
-        <v>0</v>
-      </c>
-      <c r="O8" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="P8" s="3">
+      <c r="O8" s="3">
+        <v>0</v>
+      </c>
+      <c r="P8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q8" s="3">
         <v>2</v>
       </c>
-      <c r="Q8" s="3">
-        <v>0</v>
-      </c>
       <c r="R8" s="3">
+        <v>0</v>
+      </c>
+      <c r="S8" s="3">
         <v>2</v>
       </c>
-      <c r="S8" s="3">
+      <c r="T8" s="3">
         <v>3</v>
       </c>
-      <c r="T8" s="3">
-        <v>1</v>
-      </c>
       <c r="U8" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V8" s="3">
-        <v>1</v>
-      </c>
-      <c r="W8" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="W8" s="3">
         <v>1</v>
       </c>
       <c r="X8" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y8" s="3" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:24" s="3" customFormat="1" ht="33">
+    <row r="9" spans="1:25" s="3" customFormat="1" ht="33">
       <c r="A9" s="3">
         <v>10003004</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G9" s="3">
         <v>275</v>
@@ -1382,58 +1400,58 @@
       <c r="M9" s="3">
         <v>0</v>
       </c>
-      <c r="N9" s="3">
-        <v>0</v>
-      </c>
-      <c r="O9" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="P9" s="3">
+      <c r="O9" s="3">
+        <v>0</v>
+      </c>
+      <c r="P9" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q9" s="3">
         <v>50</v>
       </c>
-      <c r="Q9" s="3">
+      <c r="R9" s="3">
         <v>25</v>
       </c>
-      <c r="R9" s="3">
+      <c r="S9" s="3">
         <v>2</v>
       </c>
-      <c r="S9" s="3">
+      <c r="T9" s="3">
         <v>5</v>
       </c>
-      <c r="T9" s="3">
-        <v>1</v>
-      </c>
       <c r="U9" s="3">
+        <v>1</v>
+      </c>
+      <c r="V9" s="3">
         <v>0.2</v>
       </c>
-      <c r="V9" s="3">
+      <c r="W9" s="3">
         <v>10</v>
       </c>
-      <c r="W9" s="3" t="b">
-        <v>1</v>
-      </c>
       <c r="X9" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y9" s="3" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:24" s="3" customFormat="1" ht="33">
+    <row r="10" spans="1:25" s="3" customFormat="1" ht="33">
       <c r="A10" s="3">
         <v>10004001</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G10" s="3">
         <v>120</v>
@@ -1456,58 +1474,58 @@
       <c r="M10" s="3">
         <v>0</v>
       </c>
-      <c r="N10" s="3">
-        <v>0</v>
-      </c>
-      <c r="O10" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="P10" s="3">
+      <c r="O10" s="3">
+        <v>0</v>
+      </c>
+      <c r="P10" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q10" s="3">
         <v>5</v>
       </c>
-      <c r="Q10" s="3">
+      <c r="R10" s="3">
         <v>15</v>
       </c>
-      <c r="R10" s="3">
+      <c r="S10" s="3">
         <v>0.05</v>
-      </c>
-      <c r="S10" s="3">
-        <v>5</v>
       </c>
       <c r="T10" s="3">
         <v>5</v>
       </c>
       <c r="U10" s="3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="V10" s="3">
+        <v>1</v>
+      </c>
+      <c r="W10" s="3">
         <v>10</v>
       </c>
-      <c r="W10" s="3" t="b">
-        <v>0</v>
-      </c>
       <c r="X10" s="3" t="b">
         <v>0</v>
       </c>
+      <c r="Y10" s="3" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="11" spans="1:24" s="3" customFormat="1" ht="49.5">
+    <row r="11" spans="1:25" s="3" customFormat="1" ht="49.5">
       <c r="A11" s="3">
         <v>10004002</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G11" s="3">
         <v>200</v>
@@ -1530,58 +1548,58 @@
       <c r="M11" s="3">
         <v>0</v>
       </c>
-      <c r="N11" s="3">
-        <v>0</v>
-      </c>
-      <c r="O11" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="P11" s="3">
+      <c r="O11" s="3">
+        <v>0</v>
+      </c>
+      <c r="P11" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q11" s="3">
         <v>50</v>
       </c>
-      <c r="Q11" s="3">
+      <c r="R11" s="3">
         <v>20</v>
       </c>
-      <c r="R11" s="3">
+      <c r="S11" s="3">
         <v>0.5</v>
       </c>
-      <c r="S11" s="3">
+      <c r="T11" s="3">
         <v>5</v>
       </c>
-      <c r="T11" s="3">
-        <v>1</v>
-      </c>
       <c r="U11" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V11" s="3">
+        <v>0</v>
+      </c>
+      <c r="W11" s="3">
         <v>10</v>
       </c>
-      <c r="W11" s="3" t="b">
-        <v>0</v>
-      </c>
       <c r="X11" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="Y11" s="3" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:24" s="3" customFormat="1" ht="49.5">
+    <row r="12" spans="1:25" s="3" customFormat="1" ht="49.5">
       <c r="A12" s="3">
         <v>10004003</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="G12" s="3">
         <v>150</v>
@@ -1604,44 +1622,44 @@
       <c r="M12" s="3">
         <v>0</v>
       </c>
-      <c r="N12" s="3">
-        <v>0</v>
-      </c>
-      <c r="O12" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="P12" s="3">
+      <c r="O12" s="3">
+        <v>0</v>
+      </c>
+      <c r="P12" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q12" s="3">
         <v>125</v>
       </c>
-      <c r="Q12" s="3">
+      <c r="R12" s="3">
         <v>50</v>
       </c>
-      <c r="R12" s="3">
-        <v>0</v>
-      </c>
       <c r="S12" s="3">
+        <v>0</v>
+      </c>
+      <c r="T12" s="3">
         <v>3</v>
       </c>
-      <c r="T12" s="3">
-        <v>1</v>
-      </c>
       <c r="U12" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V12" s="3">
+        <v>0</v>
+      </c>
+      <c r="W12" s="3">
         <v>10</v>
       </c>
-      <c r="W12" s="3" t="b">
-        <v>0</v>
-      </c>
       <c r="X12" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="Y12" s="3" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:24" s="3" customFormat="1"/>
-    <row r="14" spans="1:24" s="3" customFormat="1"/>
-    <row r="15" spans="1:24" s="3" customFormat="1"/>
-    <row r="16" spans="1:24" s="3" customFormat="1"/>
+    <row r="13" spans="1:25" s="3" customFormat="1"/>
+    <row r="14" spans="1:25" s="3" customFormat="1"/>
+    <row r="15" spans="1:25" s="3" customFormat="1"/>
+    <row r="16" spans="1:25" s="3" customFormat="1"/>
     <row r="17" s="3" customFormat="1"/>
     <row r="18" s="3" customFormat="1"/>
     <row r="19" s="3" customFormat="1"/>

</xml_diff>

<commit_message>
Fix: Module Spec UI 표기 버그 수정
</commit_message>
<xml_diff>
--- a/Assets/@Project/Scripts/Data/RawData/PartDbSheet.xlsx
+++ b/Assets/@Project/Scripts/Data/RawData/PartDbSheet.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27605"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27609"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6BA135CC-9B67-4021-A206-1A438F74C2CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{331B42B1-0987-4D2E-AC01-A3940656B4A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -743,8 +743,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -960,7 +960,7 @@
         <v>38</v>
       </c>
       <c r="G3" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H3" s="5" t="b">
         <v>0</v>
@@ -1132,7 +1132,7 @@
         <v>48</v>
       </c>
       <c r="G5" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H5" s="5" t="b">
         <v>0</v>
@@ -1301,7 +1301,7 @@
         <v>59</v>
       </c>
       <c r="G7" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7" s="5" t="b">
         <v>1</v>
@@ -1384,7 +1384,7 @@
         <v>65</v>
       </c>
       <c r="G8" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8" s="5" t="b">
         <v>1</v>
@@ -1467,7 +1467,7 @@
         <v>70</v>
       </c>
       <c r="G9" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H9" s="5" t="b">
         <v>0</v>
@@ -1633,7 +1633,7 @@
         <v>82</v>
       </c>
       <c r="G11" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H11" s="5" t="b">
         <v>1</v>
@@ -1716,7 +1716,7 @@
         <v>88</v>
       </c>
       <c r="G12" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H12" s="5" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
Feat: Localization - Module 메뉴 전체
</commit_message>
<xml_diff>
--- a/Assets/@Project/Scripts/Data/RawData/PartDbSheet.xlsx
+++ b/Assets/@Project/Scripts/Data/RawData/PartDbSheet.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27615"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27618"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{370A25D4-870E-4434-9453-F41B7F5E0B03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{65151DF9-BC0C-42DC-9E96-470452AA1041}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="103">
   <si>
     <t>dev_ID</t>
   </si>
@@ -48,7 +48,10 @@
     <t>display_Name</t>
   </si>
   <si>
-    <t>display_Description</t>
+    <t>display_Description_EN</t>
+  </si>
+  <si>
+    <t>display_Description_KO</t>
   </si>
   <si>
     <t>initialPart</t>
@@ -132,7 +135,11 @@
     <t>DG-001</t>
   </si>
   <si>
-    <t>경량형 역관절 로어파츠
+    <t>[Lightweight Reverse-Jointed Lower Parts]
+Light and fast but equipped with weak armor.</t>
+  </si>
+  <si>
+    <t>[경량형 역관절 로어파츠]
 가볍고 빠르지만 빈약한 장갑</t>
   </si>
   <si>
@@ -151,7 +158,11 @@
     <t>LF_G-002</t>
   </si>
   <si>
-    <t>하이브리드 로어파츠
+    <t>[HybridLowerParts]
+Offers good durability with its thick armor but lacks in mobility.</t>
+  </si>
+  <si>
+    <t>[하이브리드 로어파츠]
 장갑이 두꺼워 내구성은 좋으나
 기동성에서 아쉬운 모습을 보인다</t>
   </si>
@@ -168,7 +179,11 @@
     <t>UH-001</t>
   </si>
   <si>
-    <t>경량형 헤드파츠
+    <t>[LightweightHeadParts]
+Fast rotation speed but lower booster charge and hovering capabilities.</t>
+  </si>
+  <si>
+    <t>[경량형 헤드파츠]
 회전속도가 빠르지만
 부스터 충전량과 호버링 출력이 떨어진다</t>
   </si>
@@ -185,7 +200,12 @@
     <t>NB_UH-003</t>
   </si>
   <si>
-    <t>중량형 헤드파츠
+    <t>[Heavy Duty Head Parts]
+Good booster charge and hovering output
+But lacking in rotation speed</t>
+  </si>
+  <si>
+    <t>[중량형 헤드파츠]
 부스터 충전량과 호버링 출력은 좋으나
 회전속도가 떨어진다</t>
   </si>
@@ -202,7 +222,11 @@
     <t>CA-STD</t>
   </si>
   <si>
-    <t>밸런스형 1연장 캐논
+    <t>[Balanced Type 1 Barrel Extension Cannon]
+Has decent firing rate and bullet convergence</t>
+  </si>
+  <si>
+    <t>[밸런스형 1연장 캐논]
 적당한 연사력과 집탄력을 가지고있다</t>
   </si>
   <si>
@@ -221,7 +245,12 @@
     <t>GA-S</t>
   </si>
   <si>
-    <t>소형 개틀링건
+    <t>[Compact Gatling Gun]
+Capable of concentrated barrage
+But not very effective against distant targets</t>
+  </si>
+  <si>
+    <t>[소형 개틀링건]
 집중포화가 가능하지만
 멀리있는 타겟에서 그다지 좋은 효과를 내진 못한다</t>
   </si>
@@ -241,7 +270,12 @@
     <t>LC-S</t>
   </si>
   <si>
-    <t>소형 레이저캐논
+    <t>[Compact Laser Cannon]
+Inflicts laser attack on single target
+Long charging and reloading times but proven firepower</t>
+  </si>
+  <si>
+    <t>[소형 레이저캐논]
 단일 타겟에 대한 레이저 공격을 가한다
 충전시간과 재장전 시간이 길지만 화력은 검증되었다</t>
   </si>
@@ -258,7 +292,11 @@
     <t>CA-AP</t>
   </si>
   <si>
-    <t>1연장 AP 캐논
+    <t>[Single Barrel Armor Piercing Cannon]
+Boasts powerful single shot but lacking in firing rate</t>
+  </si>
+  <si>
+    <t>[1연장 AP 캐논]
 강력한 한 방을 자랑하지만 연사력이 좋지않다</t>
   </si>
   <si>
@@ -277,7 +315,12 @@
     <t>RL-Rapid</t>
   </si>
   <si>
-    <t>고정형 로켓런처
+    <t>[Fixed Rocket Launcher]
+Fires 5 rockets sequentially into the air to home in on target
+Can inflict damage on enemies in small radius at explosion point</t>
+  </si>
+  <si>
+    <t>[고정형 로켓런처]
 5발을 차례로 공중으로 발사 후 타겟을 향해 유도한다
 폭발 지점 좁은 범위의 적에게 피해를 입힐 수 있다</t>
   </si>
@@ -297,7 +340,12 @@
     <t>ML-HellFire</t>
   </si>
   <si>
-    <t>2연장 미사일런처
+    <t>[Twin Barrel Missile Launcher]
+Fires medium-sized missiles loaded with high explosives
+Can inflict damage on enemies near the explosion point</t>
+  </si>
+  <si>
+    <t>[2연장 미사일런처]
 고폭탄을 적재한 중형 미사일을 발사한다
 폭발 지점 주변의 적에게 피해를 입힐 수 있다</t>
   </si>
@@ -317,7 +365,13 @@
     <t>HE-TA</t>
   </si>
   <si>
-    <t>1연장 고폭 캐논
+    <t>[Single Barrel High Explosive Cannon]
+Fires high explosive shells that inflict heavy damage
+Can damage enemies near the explosion point
+[Fires straight ahead of unit without aiming]</t>
+  </si>
+  <si>
+    <t>[1연장 고폭 캐논]
 강력한 데미지를 가하는 고폭탄을 발사한다
 폭발 지점 주변의 적에게 피해를 입힐 수 있다
 [비조준 사격 시 기체 전방으로 발사합니다.]</t>
@@ -394,7 +448,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -403,14 +457,19 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -746,10 +805,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AC22"/>
+  <dimension ref="A1:AD21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -759,22 +818,23 @@
     <col min="3" max="3" width="49.25" customWidth="1"/>
     <col min="4" max="4" width="28" customWidth="1"/>
     <col min="5" max="5" width="25.875" customWidth="1"/>
-    <col min="6" max="6" width="47.875" customWidth="1"/>
-    <col min="7" max="7" width="13.5" customWidth="1"/>
-    <col min="8" max="9" width="15.5" customWidth="1"/>
-    <col min="13" max="13" width="13.125" customWidth="1"/>
-    <col min="14" max="14" width="13" customWidth="1"/>
-    <col min="16" max="18" width="16.375" customWidth="1"/>
-    <col min="19" max="19" width="56.125" customWidth="1"/>
-    <col min="21" max="21" width="14.5" customWidth="1"/>
-    <col min="23" max="23" width="14.625" customWidth="1"/>
-    <col min="24" max="24" width="18.5" customWidth="1"/>
-    <col min="25" max="25" width="15.125" customWidth="1"/>
-    <col min="27" max="27" width="19.5" customWidth="1"/>
-    <col min="28" max="28" width="14.875" customWidth="1"/>
+    <col min="6" max="6" width="45.125" customWidth="1"/>
+    <col min="7" max="7" width="47.875" customWidth="1"/>
+    <col min="8" max="8" width="13.5" customWidth="1"/>
+    <col min="9" max="10" width="15.5" customWidth="1"/>
+    <col min="14" max="14" width="13.125" customWidth="1"/>
+    <col min="15" max="15" width="13" customWidth="1"/>
+    <col min="17" max="19" width="16.375" customWidth="1"/>
+    <col min="20" max="20" width="56.125" customWidth="1"/>
+    <col min="22" max="22" width="14.5" customWidth="1"/>
+    <col min="24" max="24" width="14.625" customWidth="1"/>
+    <col min="25" max="25" width="18.5" customWidth="1"/>
+    <col min="26" max="26" width="15.125" customWidth="1"/>
+    <col min="28" max="28" width="19.5" customWidth="1"/>
+    <col min="29" max="29" width="14.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" s="1" customFormat="1">
+    <row r="1" spans="1:30" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -862,55 +922,58 @@
       <c r="AC1" s="1" t="s">
         <v>28</v>
       </c>
+      <c r="AD1" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="2" spans="1:29" s="2" customFormat="1" ht="33">
+    <row r="2" spans="1:30" s="2" customFormat="1" ht="33">
       <c r="A2" s="2">
         <v>10001001</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="C2" s="3" t="s">
         <v>31</v>
       </c>
+      <c r="D2" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="E2" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F2" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="G2" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="H2" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="I2" s="5">
-        <v>0</v>
-      </c>
-      <c r="J2" s="2">
+      <c r="F2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="I2" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="J2" s="3">
+        <v>0</v>
+      </c>
+      <c r="K2" s="2">
         <v>1700</v>
       </c>
-      <c r="K2" s="2">
+      <c r="L2" s="2">
         <v>180</v>
       </c>
-      <c r="L2" s="2">
+      <c r="M2" s="2">
         <v>6</v>
-      </c>
-      <c r="M2" s="2">
-        <v>5</v>
       </c>
       <c r="N2" s="2">
         <v>5</v>
       </c>
-      <c r="O2" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="P2" s="2">
-        <v>0</v>
+      <c r="O2" s="2">
+        <v>5</v>
+      </c>
+      <c r="P2" s="2" t="b">
+        <v>1</v>
       </c>
       <c r="Q2" s="2">
         <v>0</v>
@@ -918,11 +981,11 @@
       <c r="R2" s="2">
         <v>0</v>
       </c>
-      <c r="S2" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="T2" s="2">
-        <v>0</v>
+      <c r="S2" s="2">
+        <v>0</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="U2" s="2">
         <v>0</v>
@@ -945,74 +1008,77 @@
       <c r="AA2" s="2">
         <v>0</v>
       </c>
-      <c r="AB2" s="2" t="b">
+      <c r="AB2" s="2">
         <v>0</v>
       </c>
       <c r="AC2" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="AD2" s="2" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:29" s="2" customFormat="1" ht="49.5">
+    <row r="3" spans="1:30" s="2" customFormat="1" ht="49.5">
       <c r="A3" s="2">
         <v>10001002</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="H3" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="I3" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="J3" s="3">
+        <v>0</v>
+      </c>
+      <c r="K3" s="2">
+        <v>2500</v>
+      </c>
+      <c r="L3" s="2">
+        <v>350</v>
+      </c>
+      <c r="M3" s="4">
+        <v>5</v>
+      </c>
+      <c r="N3" s="2">
+        <v>3</v>
+      </c>
+      <c r="O3" s="2">
+        <v>4</v>
+      </c>
+      <c r="P3" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="2">
+        <v>0</v>
+      </c>
+      <c r="R3" s="2">
+        <v>0</v>
+      </c>
+      <c r="S3" s="2">
+        <v>0</v>
+      </c>
+      <c r="T3" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="G3" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H3" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="I3" s="5">
-        <v>0</v>
-      </c>
-      <c r="J3" s="2">
-        <v>2500</v>
-      </c>
-      <c r="K3" s="2">
-        <v>350</v>
-      </c>
-      <c r="L3" s="6">
-        <v>5</v>
-      </c>
-      <c r="M3" s="2">
-        <v>3</v>
-      </c>
-      <c r="N3" s="2">
-        <v>4</v>
-      </c>
-      <c r="O3" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="P3" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="2">
-        <v>0</v>
-      </c>
-      <c r="R3" s="2">
-        <v>0</v>
-      </c>
-      <c r="S3" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="T3" s="2">
-        <v>0</v>
-      </c>
       <c r="U3" s="2">
         <v>0</v>
       </c>
@@ -1034,73 +1100,76 @@
       <c r="AA3" s="2">
         <v>0</v>
       </c>
-      <c r="AB3" s="2" t="b">
+      <c r="AB3" s="2">
         <v>0</v>
       </c>
       <c r="AC3" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="AD3" s="2" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:29" s="2" customFormat="1" ht="49.5">
+    <row r="4" spans="1:30" s="2" customFormat="1" ht="49.5">
       <c r="A4" s="2">
         <v>10002001</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="G4" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="H4" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="I4" s="5">
-        <v>0</v>
-      </c>
-      <c r="J4" s="2">
+        <v>46</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="H4" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="I4" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="J4" s="3">
+        <v>0</v>
+      </c>
+      <c r="K4" s="2">
         <v>1500</v>
       </c>
-      <c r="K4" s="2">
+      <c r="L4" s="2">
         <v>150</v>
       </c>
-      <c r="L4" s="2">
-        <v>0</v>
-      </c>
       <c r="M4" s="2">
         <v>0</v>
       </c>
       <c r="N4" s="2">
         <v>0</v>
       </c>
-      <c r="O4" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="P4" s="2">
+      <c r="O4" s="2">
+        <v>0</v>
+      </c>
+      <c r="P4" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="2">
         <v>5</v>
       </c>
-      <c r="Q4" s="2">
+      <c r="R4" s="2">
         <v>100</v>
       </c>
-      <c r="R4" s="2">
+      <c r="S4" s="2">
         <v>5</v>
       </c>
-      <c r="S4" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="T4" s="2">
-        <v>0</v>
+      <c r="T4" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="U4" s="2">
         <v>0</v>
@@ -1123,73 +1192,76 @@
       <c r="AA4" s="2">
         <v>0</v>
       </c>
-      <c r="AB4" s="2" t="b">
+      <c r="AB4" s="2">
         <v>0</v>
       </c>
       <c r="AC4" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="AD4" s="2" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:29" s="2" customFormat="1" ht="49.5">
+    <row r="5" spans="1:30" s="2" customFormat="1" ht="49.5">
       <c r="A5" s="2">
         <v>10002002</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="G5" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H5" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="I5" s="5">
-        <v>0</v>
-      </c>
-      <c r="J5" s="2">
+        <v>52</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H5" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="I5" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="J5" s="3">
+        <v>0</v>
+      </c>
+      <c r="K5" s="2">
         <v>2300</v>
       </c>
-      <c r="K5" s="2">
+      <c r="L5" s="2">
         <v>300</v>
       </c>
-      <c r="L5" s="2">
-        <v>0</v>
-      </c>
       <c r="M5" s="2">
         <v>0</v>
       </c>
       <c r="N5" s="2">
         <v>0</v>
       </c>
-      <c r="O5" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="P5" s="2">
+      <c r="O5" s="2">
+        <v>0</v>
+      </c>
+      <c r="P5" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="2">
         <v>3</v>
       </c>
-      <c r="Q5" s="2">
+      <c r="R5" s="2">
         <v>150</v>
       </c>
-      <c r="R5" s="2">
+      <c r="S5" s="2">
         <v>7</v>
       </c>
-      <c r="S5" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="T5" s="2">
-        <v>0</v>
+      <c r="T5" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="U5" s="2">
         <v>0</v>
@@ -1212,625 +1284,648 @@
       <c r="AA5" s="2">
         <v>0</v>
       </c>
-      <c r="AB5" s="2" t="b">
+      <c r="AB5" s="2">
         <v>0</v>
       </c>
       <c r="AC5" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="AD5" s="2" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:29" s="2" customFormat="1" ht="33">
+    <row r="6" spans="1:30" s="2" customFormat="1" ht="33">
       <c r="A6" s="2">
         <v>10003001</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="H6" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="I6" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="J6" s="3">
+        <v>0</v>
+      </c>
+      <c r="K6" s="2">
+        <v>350</v>
+      </c>
+      <c r="L6" s="2">
+        <v>5</v>
+      </c>
+      <c r="M6" s="2">
+        <v>0</v>
+      </c>
+      <c r="N6" s="2">
+        <v>0</v>
+      </c>
+      <c r="O6" s="2">
+        <v>0</v>
+      </c>
+      <c r="P6" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="2">
+        <v>0</v>
+      </c>
+      <c r="S6" s="2">
+        <v>0</v>
+      </c>
+      <c r="T6" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="U6" s="2">
+        <v>10</v>
+      </c>
+      <c r="V6" s="2">
         <v>50</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="G6" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="H6" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="I6" s="5">
-        <v>0</v>
-      </c>
-      <c r="J6" s="2">
-        <v>350</v>
-      </c>
-      <c r="K6" s="2">
-        <v>5</v>
-      </c>
-      <c r="L6" s="2">
-        <v>0</v>
-      </c>
-      <c r="M6" s="2">
-        <v>0</v>
-      </c>
-      <c r="N6" s="2">
-        <v>0</v>
-      </c>
-      <c r="O6" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="P6" s="2">
-        <v>0</v>
-      </c>
-      <c r="R6" s="2">
-        <v>0</v>
-      </c>
-      <c r="S6" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="T6" s="2">
-        <v>10</v>
-      </c>
-      <c r="U6" s="2">
-        <v>50</v>
-      </c>
-      <c r="V6" s="2">
+      <c r="W6" s="2">
         <v>0.3</v>
       </c>
-      <c r="W6" s="2">
+      <c r="X6" s="2">
         <v>2.5</v>
       </c>
-      <c r="X6" s="2">
-        <v>1</v>
-      </c>
       <c r="Y6" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z6" s="2">
         <v>0.5</v>
       </c>
-      <c r="Z6" s="2">
+      <c r="AA6" s="2">
         <v>30</v>
       </c>
-      <c r="AA6" s="2">
-        <v>0</v>
-      </c>
-      <c r="AB6" s="2" t="b">
-        <v>1</v>
+      <c r="AB6" s="2">
+        <v>0</v>
       </c>
       <c r="AC6" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD6" s="2" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:29" s="2" customFormat="1" ht="49.5">
+    <row r="7" spans="1:30" s="2" customFormat="1" ht="49.5">
       <c r="A7" s="2">
         <v>10003002</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>58</v>
+        <v>63</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>64</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="G7" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H7" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="I7" s="5">
+        <v>65</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="H7" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="I7" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="J7" s="3">
         <v>1000</v>
       </c>
-      <c r="J7" s="2">
+      <c r="K7" s="2">
         <v>275</v>
       </c>
-      <c r="K7" s="2">
+      <c r="L7" s="2">
         <v>10</v>
       </c>
-      <c r="L7" s="2">
-        <v>0</v>
-      </c>
       <c r="M7" s="2">
         <v>0</v>
       </c>
       <c r="N7" s="2">
         <v>0</v>
       </c>
-      <c r="O7" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="P7" s="2">
-        <v>0</v>
-      </c>
-      <c r="R7" s="2">
-        <v>0</v>
-      </c>
-      <c r="S7" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="T7" s="2">
-        <v>1</v>
+      <c r="O7" s="2">
+        <v>0</v>
+      </c>
+      <c r="P7" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="2">
+        <v>0</v>
+      </c>
+      <c r="S7" s="2">
+        <v>0</v>
+      </c>
+      <c r="T7" s="2" t="s">
+        <v>68</v>
       </c>
       <c r="U7" s="2">
+        <v>1</v>
+      </c>
+      <c r="V7" s="2">
         <v>75</v>
       </c>
-      <c r="V7" s="2">
+      <c r="W7" s="2">
         <v>0.05</v>
       </c>
-      <c r="W7" s="2">
+      <c r="X7" s="2">
         <v>5</v>
       </c>
-      <c r="X7" s="2">
-        <v>1</v>
-      </c>
       <c r="Y7" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z7" s="2">
         <v>2</v>
       </c>
-      <c r="Z7" s="2">
+      <c r="AA7" s="2">
         <v>200</v>
       </c>
-      <c r="AA7" s="2">
-        <v>0</v>
-      </c>
-      <c r="AB7" s="2" t="b">
-        <v>1</v>
+      <c r="AB7" s="2">
+        <v>0</v>
       </c>
       <c r="AC7" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD7" s="2" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:29" s="2" customFormat="1" ht="49.5">
+    <row r="8" spans="1:30" s="2" customFormat="1" ht="66">
       <c r="A8" s="2">
         <v>10003003</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>64</v>
+        <v>70</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="G8" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H8" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="I8" s="5">
+        <v>72</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H8" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="I8" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="J8" s="3">
         <v>2500</v>
       </c>
-      <c r="J8" s="2">
+      <c r="K8" s="2">
         <v>275</v>
       </c>
-      <c r="K8" s="2">
+      <c r="L8" s="2">
         <v>10</v>
       </c>
-      <c r="L8" s="2">
-        <v>0</v>
-      </c>
       <c r="M8" s="2">
         <v>0</v>
       </c>
       <c r="N8" s="2">
         <v>0</v>
       </c>
-      <c r="O8" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="P8" s="2">
-        <v>0</v>
-      </c>
-      <c r="R8" s="2">
-        <v>0</v>
-      </c>
-      <c r="S8" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="T8" s="2">
+      <c r="O8" s="2">
+        <v>0</v>
+      </c>
+      <c r="P8" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="2">
+        <v>0</v>
+      </c>
+      <c r="S8" s="2">
+        <v>0</v>
+      </c>
+      <c r="T8" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="U8" s="2">
         <v>2</v>
       </c>
-      <c r="U8" s="2">
-        <v>0</v>
-      </c>
       <c r="V8" s="2">
+        <v>0</v>
+      </c>
+      <c r="W8" s="2">
         <v>2</v>
       </c>
-      <c r="W8" s="2">
+      <c r="X8" s="2">
         <v>3</v>
       </c>
-      <c r="X8" s="2">
-        <v>1</v>
-      </c>
       <c r="Y8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA8" s="2">
-        <v>0</v>
-      </c>
-      <c r="AB8" s="2" t="b">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="AB8" s="2">
+        <v>0</v>
       </c>
       <c r="AC8" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD8" s="2" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:29" s="2" customFormat="1" ht="33">
+    <row r="9" spans="1:30" s="2" customFormat="1" ht="49.5">
       <c r="A9" s="2">
         <v>10003004</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>69</v>
+        <v>76</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>77</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="G9" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H9" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="I9" s="5">
-        <v>0</v>
-      </c>
-      <c r="J9" s="2">
+        <v>78</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="H9" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="I9" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="J9" s="3">
+        <v>0</v>
+      </c>
+      <c r="K9" s="2">
         <v>275</v>
       </c>
-      <c r="K9" s="2">
+      <c r="L9" s="2">
         <v>10</v>
       </c>
-      <c r="L9" s="2">
-        <v>0</v>
-      </c>
       <c r="M9" s="2">
         <v>0</v>
       </c>
       <c r="N9" s="2">
         <v>0</v>
       </c>
-      <c r="O9" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="P9" s="2">
-        <v>0</v>
-      </c>
-      <c r="R9" s="2">
-        <v>0</v>
-      </c>
-      <c r="S9" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="T9" s="2">
+      <c r="O9" s="2">
+        <v>0</v>
+      </c>
+      <c r="P9" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="2">
+        <v>0</v>
+      </c>
+      <c r="S9" s="2">
+        <v>0</v>
+      </c>
+      <c r="T9" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="U9" s="2">
         <v>150</v>
       </c>
-      <c r="U9" s="2">
+      <c r="V9" s="2">
         <v>60</v>
       </c>
-      <c r="V9" s="2">
+      <c r="W9" s="2">
         <v>2</v>
       </c>
-      <c r="W9" s="2">
+      <c r="X9" s="2">
         <v>5</v>
       </c>
-      <c r="X9" s="2">
-        <v>1</v>
-      </c>
       <c r="Y9" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z9" s="2">
         <v>0.2</v>
       </c>
-      <c r="Z9" s="2">
+      <c r="AA9" s="2">
         <v>5</v>
       </c>
-      <c r="AA9" s="2">
-        <v>0</v>
-      </c>
-      <c r="AB9" s="2" t="b">
-        <v>1</v>
+      <c r="AB9" s="2">
+        <v>0</v>
       </c>
       <c r="AC9" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD9" s="2" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:29" s="2" customFormat="1" ht="49.5">
+    <row r="10" spans="1:30" s="2" customFormat="1" ht="82.5">
       <c r="A10" s="2">
         <v>10004001</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="G10" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="H10" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="I10" s="5">
-        <v>0</v>
-      </c>
-      <c r="J10" s="2">
+        <v>85</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="H10" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="I10" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="J10" s="3">
+        <v>0</v>
+      </c>
+      <c r="K10" s="2">
         <v>120</v>
       </c>
-      <c r="K10" s="2">
+      <c r="L10" s="2">
         <v>5</v>
       </c>
-      <c r="L10" s="2">
-        <v>0</v>
-      </c>
       <c r="M10" s="2">
         <v>0</v>
       </c>
       <c r="N10" s="2">
         <v>0</v>
       </c>
-      <c r="O10" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="P10" s="2">
-        <v>0</v>
-      </c>
-      <c r="R10" s="2">
-        <v>0</v>
-      </c>
-      <c r="S10" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="T10" s="2">
+      <c r="O10" s="2">
+        <v>0</v>
+      </c>
+      <c r="P10" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="2">
+        <v>0</v>
+      </c>
+      <c r="S10" s="2">
+        <v>0</v>
+      </c>
+      <c r="T10" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="U10" s="2">
         <v>22</v>
       </c>
-      <c r="U10" s="2">
+      <c r="V10" s="2">
         <v>25</v>
       </c>
-      <c r="V10" s="2">
+      <c r="W10" s="2">
         <v>0.05</v>
-      </c>
-      <c r="W10" s="2">
-        <v>5</v>
       </c>
       <c r="X10" s="2">
         <v>5</v>
       </c>
       <c r="Y10" s="2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="Z10" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA10" s="2">
         <v>250</v>
       </c>
-      <c r="AA10" s="2">
+      <c r="AB10" s="2">
         <v>3</v>
       </c>
-      <c r="AB10" s="2" t="b">
-        <v>0</v>
-      </c>
       <c r="AC10" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD10" s="2" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:29" s="2" customFormat="1" ht="49.5">
-      <c r="A11" s="2">
+    <row r="11" spans="1:30" s="6" customFormat="1" ht="82.5">
+      <c r="A11" s="6">
         <v>10004002</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="G11" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H11" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="I11" s="5">
+      <c r="B11" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="H11" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="I11" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="J11" s="7">
         <v>1500</v>
       </c>
-      <c r="J11" s="2">
+      <c r="K11" s="6">
         <v>200</v>
       </c>
-      <c r="K11" s="2">
+      <c r="L11" s="6">
         <v>8</v>
       </c>
-      <c r="L11" s="2">
-        <v>0</v>
-      </c>
-      <c r="M11" s="2">
-        <v>0</v>
-      </c>
-      <c r="N11" s="2">
-        <v>0</v>
-      </c>
-      <c r="O11" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="P11" s="2">
-        <v>0</v>
-      </c>
-      <c r="R11" s="2">
-        <v>0</v>
-      </c>
-      <c r="S11" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="T11" s="2">
+      <c r="M11" s="6">
+        <v>0</v>
+      </c>
+      <c r="N11" s="6">
+        <v>0</v>
+      </c>
+      <c r="O11" s="6">
+        <v>0</v>
+      </c>
+      <c r="P11" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="6">
+        <v>0</v>
+      </c>
+      <c r="S11" s="6">
+        <v>0</v>
+      </c>
+      <c r="T11" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="U11" s="6">
         <v>60</v>
       </c>
-      <c r="U11" s="2">
+      <c r="V11" s="6">
         <v>20</v>
       </c>
-      <c r="V11" s="2">
+      <c r="W11" s="6">
         <v>0.5</v>
       </c>
-      <c r="W11" s="2">
+      <c r="X11" s="6">
         <v>5</v>
       </c>
-      <c r="X11" s="2">
+      <c r="Y11" s="6">
         <v>2</v>
       </c>
-      <c r="Y11" s="2">
-        <v>0</v>
-      </c>
-      <c r="Z11" s="2">
+      <c r="Z11" s="6">
+        <v>0</v>
+      </c>
+      <c r="AA11" s="6">
         <v>100</v>
       </c>
-      <c r="AA11" s="2">
+      <c r="AB11" s="6">
         <v>13</v>
       </c>
-      <c r="AB11" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="AC11" s="2" t="b">
+      <c r="AC11" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD11" s="6" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:29" s="2" customFormat="1" ht="66">
+    <row r="12" spans="1:30" s="2" customFormat="1" ht="66">
       <c r="A12" s="2">
         <v>10004003</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>85</v>
+        <v>96</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="G12" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H12" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="I12" s="5">
-        <v>0</v>
-      </c>
-      <c r="J12" s="2">
+        <v>99</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="H12" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="I12" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="J12" s="3">
+        <v>0</v>
+      </c>
+      <c r="K12" s="2">
         <v>150</v>
       </c>
-      <c r="K12" s="2">
+      <c r="L12" s="2">
         <v>10</v>
       </c>
-      <c r="L12" s="2">
-        <v>0</v>
-      </c>
       <c r="M12" s="2">
         <v>0</v>
       </c>
       <c r="N12" s="2">
         <v>0</v>
       </c>
-      <c r="O12" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="P12" s="2">
-        <v>0</v>
-      </c>
-      <c r="R12" s="2">
-        <v>0</v>
-      </c>
-      <c r="S12" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="T12" s="2">
+      <c r="O12" s="2">
+        <v>0</v>
+      </c>
+      <c r="P12" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="2">
+        <v>0</v>
+      </c>
+      <c r="S12" s="2">
+        <v>0</v>
+      </c>
+      <c r="T12" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="U12" s="2">
         <v>125</v>
       </c>
-      <c r="U12" s="2">
+      <c r="V12" s="2">
         <v>100</v>
       </c>
-      <c r="V12" s="2">
-        <v>0</v>
-      </c>
       <c r="W12" s="2">
+        <v>0</v>
+      </c>
+      <c r="X12" s="2">
         <v>3</v>
       </c>
-      <c r="X12" s="2">
-        <v>1</v>
-      </c>
       <c r="Y12" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z12" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA12" s="2">
         <v>50</v>
       </c>
-      <c r="AA12" s="2">
+      <c r="AB12" s="2">
         <v>8</v>
       </c>
-      <c r="AB12" s="2" t="b">
-        <v>0</v>
-      </c>
       <c r="AC12" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD12" s="2" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:29" s="3" customFormat="1"/>
-    <row r="14" spans="1:29" s="3" customFormat="1"/>
-    <row r="15" spans="1:29" s="3" customFormat="1"/>
-    <row r="16" spans="1:29" s="3" customFormat="1"/>
-    <row r="17" s="3" customFormat="1"/>
-    <row r="18" s="3" customFormat="1"/>
-    <row r="19" s="3" customFormat="1"/>
-    <row r="20" s="3" customFormat="1"/>
-    <row r="21" s="3" customFormat="1"/>
-    <row r="22" s="4" customFormat="1"/>
+    <row r="13" spans="1:30" s="5" customFormat="1"/>
+    <row r="14" spans="1:30" s="5" customFormat="1"/>
+    <row r="15" spans="1:30" s="5" customFormat="1"/>
+    <row r="16" spans="1:30" s="5" customFormat="1"/>
+    <row r="17" s="5" customFormat="1"/>
+    <row r="18" s="5" customFormat="1"/>
+    <row r="19" s="5" customFormat="1"/>
+    <row r="20" s="5" customFormat="1"/>
+    <row r="21" s="5" customFormat="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>